<commit_message>
Add Jupyter notebook for updating log analysis tracker with results
</commit_message>
<xml_diff>
--- a/data/log_analysis_tracker.xlsx
+++ b/data/log_analysis_tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,15 +441,30 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>analysis_results_20250501</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>analysis_results_20250430</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>analysis_results_20250429</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>project</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>department</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>job_name</t>
         </is>
@@ -463,15 +478,30 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>error</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>error</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>error</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>marketing</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>campaigns</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>job_segment_users</t>
         </is>
@@ -485,15 +515,30 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>marketing</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>campaigns</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>job_update_crm</t>
         </is>
@@ -507,15 +552,30 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>marketing</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>campaigns</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>job_email_blast</t>
         </is>
@@ -529,15 +589,30 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>marketing</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>analytics</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>job_web_traffic</t>
         </is>
@@ -551,15 +626,30 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>error</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>error</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>error</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>marketing</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>analytics</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>job_conversion_rate</t>
         </is>
@@ -573,15 +663,30 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>marketing</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>analytics</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>job_roi_report</t>
         </is>
@@ -595,15 +700,30 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>finance</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>reporting</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>job_report_daily</t>
         </is>
@@ -617,15 +737,30 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>error</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>error</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>error</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>finance</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>reporting</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>job_report_weekly</t>
         </is>
@@ -639,15 +774,30 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
           <t>finance</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>reporting</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>job_report_monthly</t>
         </is>
@@ -661,15 +811,30 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>error</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>error</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>error</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
           <t>finance</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>billing</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>job_payment_proc</t>
         </is>
@@ -683,15 +848,30 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
           <t>finance</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>billing</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>job_tax_calc</t>
         </is>
@@ -705,15 +885,30 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
           <t>finance</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>billing</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>job_invoice_gen</t>
         </is>

</xml_diff>

<commit_message>
Updated log_analyzer.py to load environment variables using load_dotenv for improved configuration management. Added the addtional domain/subdomain to the tracker.
</commit_message>
<xml_diff>
--- a/data/log_analysis_tracker.xlsx
+++ b/data/log_analysis_tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,40 +441,20 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>analysis_results_20250504</t>
+          <t>analysis_results_20250505</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>analysis_results_20250503</t>
+          <t>project</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>analysis_results_20250501</t>
+          <t>department</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>analysis_results_20250430</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>analysis_results_20250429</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>project</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>department</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>job_name</t>
         </is>
@@ -483,54 +463,34 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>/logs/marketing/campaigns/job_segment_users</t>
+          <t>/logs/operations/scheduling/job_maintenance_plan</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>error</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>operations</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>error</t>
+          <t>scheduling</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>error</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>error</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>marketing</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>campaigns</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>job_segment_users</t>
+          <t>job_maintenance_plan</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>/logs/marketing/campaigns/job_update_crm</t>
+          <t>/logs/operations/scheduling/job_staff_roster</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -540,44 +500,24 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>operations</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>scheduling</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>success</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>success</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>marketing</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>campaigns</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>job_update_crm</t>
+          <t>job_staff_roster</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>/logs/marketing/campaigns/job_email_blast</t>
+          <t>/logs/operations/scheduling/job_resource_alloc</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -587,44 +527,24 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>operations</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>scheduling</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>success</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>success</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>marketing</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>campaigns</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>job_email_blast</t>
+          <t>job_resource_alloc</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>/logs/marketing/analytics/job_web_traffic</t>
+          <t>/logs/operations/logistics/job_warehouse_mgmt</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -634,44 +554,24 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>error</t>
+          <t>operations</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>logistics</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>success</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>success</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>marketing</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>analytics</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>job_web_traffic</t>
+          <t>job_warehouse_mgmt</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>/logs/marketing/analytics/job_conversion_rate</t>
+          <t>/logs/operations/logistics/job_shipment_track</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -681,138 +581,78 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>error</t>
+          <t>operations</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>error</t>
+          <t>logistics</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>error</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>error</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>marketing</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>analytics</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>job_conversion_rate</t>
+          <t>job_shipment_track</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>/logs/marketing/analytics/job_roi_report</t>
+          <t>/logs/operations/logistics/job_inventory_check</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>error</t>
+          <t>success</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>operations</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>logistics</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>success</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>success</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>marketing</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>analytics</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>job_roi_report</t>
+          <t>job_inventory_check</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>/logs/finance/reporting/job_report_daily</t>
+          <t>/logs/hr/payroll/job_tax_withhold</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>error</t>
+          <t>success</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>hr</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>payroll</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>success</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>success</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>finance</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>reporting</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>job_report_daily</t>
+          <t>job_tax_withhold</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>/logs/finance/reporting/job_report_weekly</t>
+          <t>/logs/hr/payroll/job_salary_calc</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -822,44 +662,24 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>hr</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>error</t>
+          <t>payroll</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>error</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>error</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>finance</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>reporting</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>job_report_weekly</t>
+          <t>job_salary_calc</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>/logs/finance/reporting/job_report_monthly</t>
+          <t>/logs/hr/payroll/job_bonus_process</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -869,44 +689,24 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>hr</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>payroll</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>success</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>success</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>finance</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>reporting</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>job_report_monthly</t>
+          <t>job_bonus_process</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>/logs/finance/billing/job_payment_proc</t>
+          <t>/logs/hr/recruiting/job_offer_gen</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -916,44 +716,24 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>hr</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>error</t>
+          <t>recruiting</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>error</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>error</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>finance</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>billing</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>job_payment_proc</t>
+          <t>job_offer_gen</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>/logs/finance/billing/job_tax_calc</t>
+          <t>/logs/hr/recruiting/job_interview_sched</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -963,82 +743,366 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>hr</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>recruiting</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>success</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>success</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>finance</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>billing</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>job_tax_calc</t>
+          <t>job_interview_sched</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>/logs/hr/recruiting/job_candidate_screen</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>error</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>hr</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>recruiting</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>job_candidate_screen</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>/logs/marketing/campaigns/job_segment_users</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>marketing</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>campaigns</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>job_segment_users</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>/logs/marketing/campaigns/job_update_crm</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>marketing</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>campaigns</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>job_update_crm</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>/logs/marketing/campaigns/job_email_blast</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>marketing</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>campaigns</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>job_email_blast</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>/logs/marketing/analytics/job_web_traffic</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>error</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>marketing</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>analytics</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>job_web_traffic</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>/logs/marketing/analytics/job_conversion_rate</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>marketing</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>analytics</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>job_conversion_rate</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>/logs/marketing/analytics/job_roi_report</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>error</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>marketing</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>analytics</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>job_roi_report</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>/logs/finance/reporting/job_report_daily</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>error</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>finance</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>reporting</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>job_report_daily</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>/logs/finance/reporting/job_report_weekly</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>finance</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>reporting</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>job_report_weekly</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>/logs/finance/reporting/job_report_monthly</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>finance</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>reporting</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>job_report_monthly</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>/logs/finance/billing/job_payment_proc</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>finance</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>billing</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>job_payment_proc</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>/logs/finance/billing/job_tax_calc</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>finance</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>billing</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>job_tax_calc</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
           <t>/logs/finance/billing/job_invoice_gen</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>success</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>error</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>success</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>success</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>success</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
         <is>
           <t>finance</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>billing</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>job_invoice_gen</t>
         </is>

</xml_diff>